<commit_message>
Added Nimblegen parsed and unparsed file types to spreadsheet.
</commit_message>
<xml_diff>
--- a/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
+++ b/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="-80" windowWidth="24800" windowHeight="17360" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="61">
+  <si>
+    <t>TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImaGene</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOFT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parsed?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair Report TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalized Pair Report TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>* Raw files must appear in only the Array Data File column of an accompanying SDRF (if present). Derived files must appear in only the Derived Array Data File column of an accompanying SDRF (if present).</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -60,142 +104,122 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>caArray recognizes the following tab-delimited columns: GENE_EXPR_OPTION, SEQ_ID, PROBE_ID, MATCH_INDEX, PM, MM, X, Y. "&lt;GENE_EXPR_OPTION&gt;|&lt;SEQ_ID&gt;|&lt;PROBE_ID&gt;" is used to match to the PhysicalProbe name from the NDF array design.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScanArray</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw or Derived?*</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR file format version 3.0 is supported. Format is described here: http://www.moleculardevices.com/pages/software/gn_genepix_file_formats.html#gpr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomaterial-data association</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agilent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN4 and CN5 formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illumina</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Probe Profile TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genotyping processed data matrix TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Format</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provider</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Affymetrix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>TXT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ImaGene</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GEO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOFT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GSM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScanArray</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw or Derived?*</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPR file format version 3.0 is supported. Format is described here: http://www.moleculardevices.com/pages/software/gn_genepix_file_formats.html#gpr</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomaterial-data association</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agilent</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN4 and CN5 formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Illumina</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sample Probe Profile TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genotyping processed data matrix TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Format</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Provider</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Affymetrix</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>RPT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -237,10 +261,6 @@
   </si>
   <si>
     <t>Parsing details</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parsed?</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -248,6 +268,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -616,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -636,584 +662,646 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6">
-      <c r="F33" s="2" t="s">
-        <v>0</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6">
+      <c r="F36" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated file parser table to include MAGE-TAB data matrix and copy number formats.
</commit_message>
<xml_diff>
--- a/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
+++ b/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="-80" windowWidth="24800" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,231 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
+  <si>
+    <t>caArray expects the first header row to contain tab-delimited Hybridization REFs that refer to Hybridization Names in the corresponding SDRF. The rest of the file is expected to bethe following tab-delimited columns: Reporter REF (probe name), Chromosome, Position, Log2Ratio.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAGE-TAB Data Matrix (not Copy Number)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Either</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAGE-TAB Data Matrix files can represent data from any provider, and can appear in either the Array Data Matrix File (raw) or Derived Array Data Matrix File (derived) column of an accompanying SDRF.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHP (Gene expression)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHP (Genotyping)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNCHP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genepix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAGE-TAB required?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parsing details</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy Number MAGE-TAB Data Matrix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray recognizes the following tab-delimited columns: GENE_EXPR_OPTION, SEQ_ID, PROBE_ID, MATCH_INDEX, PM, MM, X, Y. "&lt;GENE_EXPR_OPTION&gt;|&lt;SEQ_ID&gt;|&lt;PROBE_ID&gt;" is used to match to the PhysicalProbe name from the NDF array design.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, gTotalProbeSignal, gTotalProbeError, gTotalGeneSignal, gTotalGeneError, gIsGeneDetected.</t>
+  </si>
+  <si>
+    <t>Nimblegen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GFF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray recognizes the following tab-delimited columns: GENE_EXPR_OPTION, SEQ_ID, PROBE_ID, MATCH_INDEX, PM, MM, X, Y. "&lt;GENE_EXPR_OPTION&gt;|&lt;SEQ_ID&gt;|&lt;PROBE_ID&gt;" is used to match to the PhysicalProbe name from the NDF array design.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScanArray</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw or Derived?*</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR file format version 3.0 is supported. Format is described here: http://www.moleculardevices.com/pages/software/gn_genepix_file_formats.html#gpr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomaterial-data association</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agilent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN4 and CN5 formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illumina</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Probe Profile TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genotyping processed data matrix TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Format</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provider</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Affymetrix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>TXT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>RPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>ImaGene</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -90,177 +309,6 @@
   </si>
   <si>
     <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, gProcessedSignal, gProcessedSigError, gMedianSignal.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, gTotalProbeSignal, gTotalProbeError, gTotalGeneSignal, gTotalGeneError, gIsGeneDetected.</t>
-  </si>
-  <si>
-    <t>Nimblegen</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GFF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray recognizes the following tab-delimited columns: GENE_EXPR_OPTION, SEQ_ID, PROBE_ID, MATCH_INDEX, PM, MM, X, Y. "&lt;GENE_EXPR_OPTION&gt;|&lt;SEQ_ID&gt;|&lt;PROBE_ID&gt;" is used to match to the PhysicalProbe name from the NDF array design.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScanArray</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw or Derived?*</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPR file format version 3.0 is supported. Format is described here: http://www.moleculardevices.com/pages/software/gn_genepix_file_formats.html#gpr</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomaterial-data association</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agilent</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN4 and CN5 formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Illumina</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sample Probe Profile TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genotyping processed data matrix TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Format</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Provider</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Affymetrix</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHP (Gene expression)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHP (Genotyping)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CNCHP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genepix</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAGE-TAB required?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parsing details</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -644,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -662,471 +710,471 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>21</v>
@@ -1134,171 +1182,213 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="F36" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated Appendix with MAGE-TAB Data Matrix and Copy Number file/parser details.
</commit_message>
<xml_diff>
--- a/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
+++ b/end_user_documentation/working_copies/user_guide/draft_chapters/caArray_file_import.xlsx
@@ -21,7 +21,183 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
   <si>
-    <t>caArray expects the first header row to contain tab-delimited Hybridization REFs that refer to Hybridization Names in the corresponding SDRF. The rest of the file is expected to bethe following tab-delimited columns: Reporter REF (probe name), Chromosome, Position, Log2Ratio.</t>
+    <t>caArray parses several tab-delimited columns: Probe_ID/ID_REF is mandatory if the corresponding array design is in BGX/TXT format; otherwise, TargetID (mandatory) and ProbeId are expected. The following columns are present for each hybridization: AVG_Signal (mandatory), MIN_Signal, MAX_Signal, NARRAYS, ARRAY_STDEV, BEAD_STDEV, Avg_NBEADS, Detection/DetectionPval/Detection Pval (mandatory). These columns will be either prefixed with "&lt;hybridization_name&gt;." or suffixed with "-&lt;hybridization_name&gt;". Multiple hybridizations are typically represented in a single file.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray parses the following tab-delimited columns:IlmnID/ID/ID_REF (mandatory), &lt;hybridization_name&gt; (mandatory), GC_SCORE, Theta, R, B_Allele_Freq, Log_R_Ratio. The last 5 quantitation types can optionally be prefixed with "&lt;hybridization_name&gt;.". Multiple hybridizations are typically represented in a single file.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT (1-colour gene expression)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT (miRNA)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, LogRatio, LogRatioError, PValueLogRatio, gProcessedSignal, rProcessedSignal, gProcessedSigError, rProcessedSigError, gMedianSignal, rMedianSignal.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, gProcessedSignal, gProcessedSigError, gMedianSignal.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caArray expects the first header row to contain tab-delimited Hybridization REFs that refer to Hybridization Names in the corresponding SDRF. The rest of the file is expected to contain the following tab-delimited columns: Reporter REF (probe name), Chromosome, Position, Log2Ratio.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomaterial-data association</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agilent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN4 and CN5 formats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illumina</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample Probe Profile TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genotyping processed data matrix TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derived</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Format</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provider</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Affymetrix</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImaGene</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TIF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOFT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parsed?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pair Report TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalized Pair Report TXT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Raw files must appear in only the Array Data File column of an accompanying SDRF (if present). Derived files must appear in only the Derived Array Data File column of an accompanying SDRF (if present).</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -133,182 +309,6 @@
   </si>
   <si>
     <t>GPR file format version 3.0 is supported. Format is described here: http://www.moleculardevices.com/pages/software/gn_genepix_file_formats.html#gpr</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>If the data files are imported without an accompanying MAGE-TAB file set, then biomaterial-hybridization chains will be auto-generated according to the hybridization names present in the data files themselves. If accompanied by MAGE-TAB, hybridization names in SDRF will be checked against hybridization names within the data files - if the SDRF is missing one or more of the hybridization names in the data files, validation/import will fail.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomaterial-data association</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agilent</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT (aCGH and 2-colour gene expression)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; MAS5 and RMA/PLIER algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GCOS binary/XDA and Command Console/AGCC/Calvin formats; Birdseed, BRLMM and Axiom GT algorithms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN4 and CN5 formats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Illumina</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sample Probe Profile TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genotyping processed data matrix TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Derived</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Format</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Provider</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Affymetrix</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ImaGene</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GEO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOFT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GSM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parsed?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pair Report TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normalized Pair Report TXT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>* Raw files must appear in only the Array Data File column of an accompanying SDRF (if present). Derived files must appear in only the Derived Array Data File column of an accompanying SDRF (if present).</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray parses several tab-delimited columns: Probe_ID/ID_REF is mandatory if the corresponding array design is in BGX/TXT format; otherwise, TargetID (mandatory) and ProbeId are expected. The following columns are present for each hybridization: AVG_Signal (mandatory), MIN_Signal, MAX_Signal, NARRAYS, ARRAY_STDEV, BEAD_STDEV, Avg_NBEADS, Detection/DetectionPval/Detection Pval (mandatory). These columns will be either prefixed with "&lt;hybridization_name&gt;." or suffixed with "-&lt;hybridization_name&gt;". Multiple hybridizations are typically represented in a single file.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray parses the following tab-delimited columns:IlmnID/ID/ID_REF (mandatory), &lt;hybridization_name&gt; (mandatory), GC_SCORE, Theta, R, B_Allele_Freq, Log_R_Ratio. The last 5 quantitation types can optionally be prefixed with "&lt;hybridization_name&gt;.". Multiple hybridizations are typically represented in a single file.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT (1-colour gene expression)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Raw TXT (miRNA)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, LogRatio, LogRatioError, PValueLogRatio, gProcessedSignal, rProcessedSignal, gProcessedSigError, rProcessedSigError, gMedianSignal, rMedianSignal.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>caArray parses the FEATURES section of this file, and recognizes the following tab-delimited columns: ProbeName, gProcessedSignal, gProcessedSigError, gMedianSignal.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -316,12 +316,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -692,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -710,688 +704,687 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="F36" s="2" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>